<commit_message>
booking page and cart page working fine
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/A2A_Booking.xlsx
+++ b/src/main/java/com/crm/qa/testdata/A2A_Booking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devendra.singh1\git\Kargo360\src\main\java\com\crm\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishal.jain\git\Kargo360tech2025\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1985,9 +1985,7 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>